<commit_message>
new results and configs
</commit_message>
<xml_diff>
--- a/scripts/strategy_tester/results/20181201_20190131-sar-ltc_usd/Test Analysis.xlsx
+++ b/scripts/strategy_tester/results/20181201_20190131-sar-ltc_usd/Test Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software Development\zenbot\scripts\strategy_tester\results\20181201_20190131-sar-ltc_usd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6C5903-E463-4F00-ADB3-9E56EE0C7B31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209EF9B0-8BC9-4354-8AA1-B7BA48AB581D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="86280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CB0850FA-7F57-43D0-9DF3-B242DEA91448}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB0850FA-7F57-43D0-9DF3-B242DEA91448}"/>
   </bookViews>
   <sheets>
     <sheet name="dez-2018" sheetId="2" r:id="rId1"/>
@@ -10442,9 +10442,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -10458,6 +10455,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10503,9 +10503,9 @@
     <sortCondition descending="1" ref="A1"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D27BB095-BE6A-452D-B212-C6B1EF1C1F72}" uniqueName="1" name="Percent" queryTableFieldId="1" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{D27BB095-BE6A-452D-B212-C6B1EF1C1F72}" uniqueName="1" name="Percent" queryTableFieldId="1" dataDxfId="5" dataCellStyle="Percent"/>
     <tableColumn id="2" xr3:uid="{D15674C1-8909-4E4D-8AF0-C21F02B577BF}" uniqueName="2" name="WinLoss" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{3040ED25-3E82-422D-A6C7-B8B8E17BB8F9}" uniqueName="3" name="StrategyProcess" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{3040ED25-3E82-422D-A6C7-B8B8E17BB8F9}" uniqueName="3" name="StrategyProcess" queryTableFieldId="3" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10518,9 +10518,9 @@
     <sortCondition descending="1" ref="A1"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F0D8BD49-CAEC-416E-8BC5-FB1D07CBD423}" uniqueName="1" name="Percent" queryTableFieldId="1" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{F0D8BD49-CAEC-416E-8BC5-FB1D07CBD423}" uniqueName="1" name="Percent" queryTableFieldId="1" dataDxfId="2" dataCellStyle="Percent"/>
     <tableColumn id="2" xr3:uid="{19587FB4-B3B7-4690-A8A3-57CDE0E9C5C6}" uniqueName="2" name="WinLoss" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{847250D2-9F68-4CF8-8B5F-8335401321EA}" uniqueName="3" name="StrategyProcess" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{847250D2-9F68-4CF8-8B5F-8335401321EA}" uniqueName="3" name="StrategyProcess" queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10825,8 +10825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA97A583-84BA-4D6D-BE3D-EC0CADB5665B}">
   <dimension ref="A1:C1681"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29339,7 +29339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD67D27-7B24-4D5F-8488-E8A59415592F}">
   <dimension ref="A1:C1681"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>